<commit_message>
Updated progress xlsx  and minor adjustments to mapping documents
</commit_message>
<xml_diff>
--- a/Mappings/LaboratoriumResultaat - STU3.xlsx
+++ b/Mappings/LaboratoriumResultaat - STU3.xlsx
@@ -756,30 +756,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -837,6 +813,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1110,7 +1110,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1130,7 +1130,7 @@
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.140625" style="52" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1139,15 +1139,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1160,17 +1160,17 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="24"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="51" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="43" t="s">
         <v>68</v>
       </c>
       <c r="K2" s="3"/>
@@ -1181,10 +1181,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="60"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1192,31 +1192,31 @@
       <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="44" t="s">
         <v>71</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="44" customFormat="1">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41" t="s">
+    <row r="4" spans="1:12" s="36" customFormat="1">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="39" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="37" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1225,10 +1225,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -1236,7 +1236,7 @@
       <c r="I5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="46" t="s">
         <v>72</v>
       </c>
       <c r="K5" s="27" t="s">
@@ -1251,10 +1251,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -1262,7 +1262,7 @@
       <c r="I6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="55" t="s">
+      <c r="J6" s="47" t="s">
         <v>91</v>
       </c>
       <c r="K6" s="27" t="s">
@@ -1274,16 +1274,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="31"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
       <c r="I7" s="14"/>
-      <c r="J7" s="56" t="s">
+      <c r="J7" s="48" t="s">
         <v>61</v>
       </c>
       <c r="K7" s="13"/>
@@ -1304,7 +1304,7 @@
       <c r="I8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="57" t="s">
+      <c r="J8" s="49" t="s">
         <v>94</v>
       </c>
       <c r="K8" s="13"/>
@@ -1325,7 +1325,7 @@
       <c r="I9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="47" t="s">
         <v>58</v>
       </c>
       <c r="K9" s="27" t="s">
@@ -1348,7 +1348,7 @@
       <c r="I10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="55" t="s">
+      <c r="J10" s="47" t="s">
         <v>93</v>
       </c>
       <c r="K10" s="13"/>
@@ -1369,7 +1369,7 @@
       <c r="I11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="55" t="s">
+      <c r="J11" s="47" t="s">
         <v>95</v>
       </c>
       <c r="K11" s="13"/>
@@ -1390,7 +1390,7 @@
       <c r="I12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="55" t="s">
+      <c r="J12" s="47" t="s">
         <v>96</v>
       </c>
       <c r="K12" s="13"/>
@@ -1411,10 +1411,10 @@
       <c r="I13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="54" t="s">
+      <c r="J13" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="K13" s="46" t="s">
+      <c r="K13" s="38" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1423,16 +1423,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="58" t="s">
+      <c r="J14" s="50" t="s">
         <v>62</v>
       </c>
       <c r="K14" s="26"/>
@@ -1453,7 +1453,7 @@
       <c r="I15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="55" t="s">
+      <c r="J15" s="47" t="s">
         <v>99</v>
       </c>
       <c r="K15" s="13"/>
@@ -1474,7 +1474,7 @@
       <c r="I16" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="59" t="s">
+      <c r="J16" s="51" t="s">
         <v>100</v>
       </c>
       <c r="K16" s="22"/>
@@ -1486,7 +1486,7 @@
       <c r="I17" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="55" t="s">
+      <c r="J17" s="47" t="s">
         <v>101</v>
       </c>
       <c r="K17" s="29" t="s">
@@ -1500,7 +1500,7 @@
       <c r="I18" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="J18" s="55" t="s">
+      <c r="J18" s="47" t="s">
         <v>102</v>
       </c>
       <c r="K18" s="29" t="s">
@@ -1514,7 +1514,7 @@
       <c r="I19" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="J19" s="55" t="s">
+      <c r="J19" s="47" t="s">
         <v>103</v>
       </c>
       <c r="K19" s="29" t="s">
@@ -1557,19 +1557,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="48"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49" t="s">
+      <c r="A1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="48"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" ht="33.950000000000003" customHeight="1">
       <c r="A2" t="s">
@@ -1581,7 +1581,7 @@
       <c r="C2" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="42" t="s">
         <v>56</v>
       </c>
       <c r="E2" t="s">
@@ -1604,7 +1604,7 @@
       <c r="C3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="42" t="s">
         <v>51</v>
       </c>
       <c r="E3" t="s">
@@ -1627,7 +1627,7 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="42" t="s">
         <v>52</v>
       </c>
       <c r="E4" t="s">
@@ -1650,7 +1650,7 @@
       <c r="C5" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="42" t="s">
         <v>54</v>
       </c>
       <c r="E5" t="s">
@@ -1673,7 +1673,7 @@
       <c r="C6" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="42" t="s">
         <v>53</v>
       </c>
       <c r="E6" t="s">

</xml_diff>